<commit_message>
minimal change in Timerecord
</commit_message>
<xml_diff>
--- a/documents/time-records/Ertel_Bernhard_csar8812.xlsx
+++ b/documents/time-records/Ertel_Bernhard_csar8812.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t xml:space="preserve">webSockets erweitern auf cubeFace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Workshop</t>
   </si>
   <si>
     <t xml:space="preserve">Workshop Tests</t>
@@ -476,10 +473,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C45" activeCellId="0" sqref="C45"/>
+      <selection pane="bottomRight" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.13"/>
@@ -655,7 +652,7 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>17</v>
@@ -668,11 +665,11 @@
       <c r="B13" s="8" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,10 +691,10 @@
         <v>0.125</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,7 +708,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,7 +736,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,7 +750,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,7 +764,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -778,10 +775,10 @@
         <v>0.0416666666666667</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,10 +789,10 @@
         <v>0.0625</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -809,7 +806,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,7 +820,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -837,7 +834,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,13 +842,13 @@
         <v>44328</v>
       </c>
       <c r="B26" s="8" t="n">
-        <v>0.000694444444444444</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -865,7 +862,7 @@
         <v>7</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,7 +876,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,7 +890,7 @@
         <v>9</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,10 +901,10 @@
         <v>0.0625</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,7 +918,7 @@
         <v>7</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -932,10 +929,10 @@
         <v>0.0625</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,10 +943,10 @@
         <v>0.104166666666667</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,10 +957,10 @@
         <v>0.0416666666666667</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,7 +974,7 @@
         <v>7</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,7 +988,7 @@
         <v>9</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1005,7 +1002,7 @@
         <v>7</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,7 +1016,7 @@
         <v>9</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,10 +1027,10 @@
         <v>0.104166666666667</v>
       </c>
       <c r="C39" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,10 +1041,10 @@
         <v>0.104166666666667</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,7 +1058,7 @@
         <v>7</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,10 +1069,10 @@
         <v>0.166666666666667</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,10 +1083,10 @@
         <v>0.104166666666667</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,10 +1097,10 @@
         <v>0.104166666666667</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,10 +1111,10 @@
         <v>0.125</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,7 +1128,7 @@
         <v>7</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6900,7 +6897,7 @@
       <formula1>Tätigkeiten!$B$2:$B$12</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C3 C6:C8 C11:C12 C14 C16 C21:C22 C26 C28 C30 C32:C34" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C3 C6:C8 C11:C14 C16 C21:C22 C26 C28 C30 C32:C34" type="list">
       <formula1>Tätigkeiten!$B$2:$B$12</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6930,17 +6927,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6948,7 +6945,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6956,7 +6953,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6964,7 +6961,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6972,7 +6969,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6980,7 +6977,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7012,7 +7009,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7020,7 +7017,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>